<commit_message>
100m (F) Final Results
</commit_message>
<xml_diff>
--- a/SCRC_2024_Olympics_Pool_Results.xlsx
+++ b/SCRC_2024_Olympics_Pool_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67bd65b767a0c66b/Documents/SCRC Olympics PICKS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{FAA18E0E-7D27-4548-B0CF-C723337997DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{008070EB-F02B-495D-AAF0-8A995740986F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2FAB5D-7315-4CD5-AE27-85A25ADC6496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{E47C71D3-D171-487D-83A7-BB4DEDD9BAB4}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E47C71D3-D171-487D-83A7-BB4DEDD9BAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Event</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>3rd Place</t>
+  </si>
+  <si>
+    <t>Julien Alfred</t>
+  </si>
+  <si>
+    <t>Sha'Carri Richardson</t>
+  </si>
+  <si>
+    <t>Melissa Jefferson</t>
   </si>
 </sst>
 </file>
@@ -275,30 +284,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,10 +334,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -640,93 +656,101 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
400m (M) results added
</commit_message>
<xml_diff>
--- a/SCRC_2024_Olympics_Pool_Results.xlsx
+++ b/SCRC_2024_Olympics_Pool_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67bd65b767a0c66b/Documents/SCRC Olympics PICKS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncornish\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{FAA18E0E-7D27-4548-B0CF-C723337997DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DEDE08A-4511-48EE-9248-EB747AD9519D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BF6A69-3353-4FD2-B35A-D914EBE5B2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{E47C71D3-D171-487D-83A7-BB4DEDD9BAB4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E47C71D3-D171-487D-83A7-BB4DEDD9BAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Event</t>
   </si>
@@ -74,6 +74,21 @@
     <t>3rd Place</t>
   </si>
   <si>
+    <t>Gabrielle Thomas</t>
+  </si>
+  <si>
+    <t>Julien Alfred</t>
+  </si>
+  <si>
+    <t>Brittany Brown</t>
+  </si>
+  <si>
+    <t>Melissa Jefferson</t>
+  </si>
+  <si>
+    <t>Sha'Carri Richardson</t>
+  </si>
+  <si>
     <t>Noah Lyles</t>
   </si>
   <si>
@@ -83,26 +98,20 @@
     <t>Fred Kerley</t>
   </si>
   <si>
-    <t>Julien Alfred</t>
-  </si>
-  <si>
-    <t>Melissa Jefferson</t>
-  </si>
-  <si>
-    <t>Sha'Carri Richardson</t>
-  </si>
-  <si>
-    <t>Gabrielle Thomas</t>
-  </si>
-  <si>
-    <t>Brittany Brown</t>
+    <t>Quincy Hall</t>
+  </si>
+  <si>
+    <t>Mattew Hudson-Smith</t>
+  </si>
+  <si>
+    <t>Muzala Samukonga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,16 +120,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -299,30 +300,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,10 +353,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -664,19 +675,20 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -689,87 +701,93 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>